<commit_message>
Get daily reddit data: Tue Mar  5 08:08:48 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_10.xlsx
+++ b/data/2024_03_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C447"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2488 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1b6zouo</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Bling bling nude french nails😍🥰✨✨</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6zouo/bling_bling_nude_french_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1b6zno4</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Ohora/Zinnipin gellight over dip powder base?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6zno4/ohorazinnipin_gellight_over_dip_powder_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1b6x5ho</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>How to avoid torn cuticles?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6x5ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1b6w07y</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Did one of my besties’ nails in the school bathroom. They live them, I think I did pretty good for my first extensions l.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6w07y</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1b6xqwy</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Gel X - so proud of these!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjmxrczrdgmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1b6xq7s</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I did last week. </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g9h81rldgmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1b6wcpg</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Dark manicure 🖤🕸️</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxrc0b9i0gmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1b6wa0q</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Think I've got gels down. 3rd attempt</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6wa0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1b6vs22</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>so fresh n so clean clean 🌟</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kk5gancvfmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1b6qf51</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>fill in question</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6qf51/fill_in_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1b6vgtg</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Out of my comfort zone</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4ltw4zmsfmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1b6uyri</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>What can I do better?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wikxsweofmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1b6uoxo</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>“Same but different” quartz nails I’ve done the last few weeks!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6uoxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1b6ulvn</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Made &amp; Applied a set of gel press ons for my grandma🥹🖤</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbyzgjdflfmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1b6u47e</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Does anybody know of a polish this color?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6inua7ihfmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1b6tno3</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Cherry on top! Simple art for my nails today 💕</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hoqhj22odfmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1b6t5o7</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>how we feeling abt my next set?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6t5o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1b6sxse</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Some shimmer for a date night</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xesx76v7fmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1b6ssoa</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Wife's new set. It's her birthday month</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ssoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1b6sr8b</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>How much does a mani pedi run you?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6sr8b/how_much_does_a_mani_pedi_run_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1b6sj01</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Practicing</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cntehfwh4fmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1b6qxwp</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>OPI- You’ve Got that Glas-glow</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6qxwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1b6que5</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Springy nails! 🌸 🩷 🐰 </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hgs8emcremc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1b6qt6c</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>My French pedi</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skkofbj4remc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1b6qpkr</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>I need an update in latest on non gel, non dip, non acrylic nails after a decade of doing just plain polishes</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6qpkr/i_need_an_update_in_latest_on_non_gel_non_dip_non/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1b6qh4s</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>I cut my nails so I could practice solid gel extensions! What so you all think?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7u3go3eloemc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1b6pwvd</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Best desk lamp?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6pwvd/best_desk_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1b6psuq</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Spring Gel Manicure 🌸🐰🪻🌼🌷</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkc5iwqkjemc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1b6p78w</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>My first time trying to do ombre nails</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6p78w</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1b6obcy</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Boy nails!!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6v7bxl69emc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1b6nzuh</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>My first time getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7kqch2x6emc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1b6nvsj</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Service needed</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6nvsj/service_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1b6noyy</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Feeling like catwoman in the best way after fresh set :-))</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6noyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1b6kyti</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Can someone help me find this gel polish?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6kyti</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1b6nhib</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Purple Rain ☔️</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6nhib</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1b6mpuf</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>DIY press on</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40vqzzesxdmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1b6mpas</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>My very first at-home hard gels!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6mpas/my_very_first_athome_hard_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1b6m9sp</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>First spring set of the year 🌸</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6m9sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1b6lwo4</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Got super long ones done for the first time!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57m98ji0sdmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1b6lc9r</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Red underneath and black on top makes me feel like I have Louboutins on lol</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuvv2wnyndmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1b6lbot</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I'm obsessed!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6lbot</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1b6lbjk</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>New nails, who dis</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6lbjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1b6l65j</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polygel nails </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb95yfxqmdmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1b6l32i</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Chrome or Unicorn?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcor4nv4mdmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1b6kmux</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Hand painted Pastel Sparkle</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6kmux</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1b6kixi</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Tough on nails - what sticks?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6kixi/tough_on_nails_what_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1b6jw2p</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>orange chrome &amp; flames for my birthday 🔥♈️</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er583iujddmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1b6jefy</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Simply Black🖤</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdgtgco1admc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1b6izxd</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Is there a way to get less crud under your nails as you go about your day?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6izxd/is_there_a_way_to_get_less_crud_under_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1b6iy9t</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vacation nails </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axs011ps6dmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1b6id8q</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm really in love </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7tskk0n2dmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1b6hz22</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Best method for oil soaks</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6hz22/best_method_for_oil_soaks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1b6heej</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>My one week old structured mani on myself.</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj5aedzuvcmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1b6h0xn</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Expressie streaky? </t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6h0xn/essie_expressie_streaky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1b6gzjn</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Spring nails because we’ve had 70° weather in WI</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v88wi2zscmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1b6gugp</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>First Time Painting My Nails!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/faas0hn0scmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1b6gu1b</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>2 week update</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6gu1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1b6fwbz</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>New to nail salons</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6fwbz/new_to_nail_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1b6gbls</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Best way to remove acrylics?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6gbls/best_way_to_remove_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1b6g6ql</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Dichroic glass effect nails 🔷</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frx8tjthncmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1b6foke</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I’m 37 and this is my first manicure ever! Green for St.Pattys day</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtifbetyjcmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1b6cpra</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>I recreated a set I saw on Pinterest on myself :)</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g53v558tybmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1b6a722</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Containing monomer smell </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://a.co/d/fboB7Sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1b6fa19</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>first spring nails🪷love these so much!!!!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzf9ogf1hcmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1b6f8gz</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>It's amazing what a minimal pop of color can do to boost your mood!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zhqo8urgcmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1b63hlc</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Crises on nails</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t28vf6mlb9mc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1b61o3g</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Does anyone know how to get this done? (Original by @yuri_sorally on IG)</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4khnydcyt8mc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1b6erhb</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Chipped gel polish</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfxxaw1gdcmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1b6dy88</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Bi guy wanting to show my pride for myself</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6dy88/bi_guy_wanting_to_show_my_pride_for_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1b6d1wm</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Nail stickers</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6d1wm</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1b6cv5p</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Moody nails cause I'm a moody bishh</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q35dfvzvzbmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1b6btvh</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Obsessed with sparkles lately✨</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rne2c3i2sbmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1b6b3p9</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>✨️✨️✨️</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8gqatg8mbmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1b6askd</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Cat Eye ✨</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0lqvy2jjbmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1b6aet9</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Nail Glue</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b6aet9/nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1b69xp2</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Affordable base coat recommendations?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b69xp2/affordable_base_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1b69wvi</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b69wvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1b69wot</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Lilac is my pasión!</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0ga5mrbbbmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1b69vgk</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>My first time sculpting my own charms!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqjshezzabmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1b69eu9</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gypn6mwi6bmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1b6951i</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st time using UV nail stickers + a small layer of UV resin to add a dried flower </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p73iaafw3bmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1b68vbh</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Fake hand nails on wide thumbs</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b68vbh/fake_hand_nails_on_wide_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1b68aii</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>pink and glitter</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b68aii</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1b67pby</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Magnetic gel</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fyrokdawnamc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1b67fhi</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>My progress</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b67fhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1b7006o</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Confused and disappointed?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7006o</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1b6wyfr</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Improved on my nails inspired by the matrix!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvolnp976gmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1b6woe1</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Day 1 vs Day 3?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6woe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1b6waym</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Bad batch?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b6waym/bad_batch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1b6uqud</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>More Fun with Magnets</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6uqud</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1b6ugn1</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>March obsession : Poison Ivy’s Toxic Kiss - Danglefoot Nail Polish - January PPU 24’</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ugn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1b6ty5v</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Fancy Chameleon</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ty5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1b6so0i</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So many people seem to love holo taco. I bought a bunch over the past few months because of the great things I heard.  I was painting my nails tonight with foiled again for St Patrick's Day. It was gloppy &amp; not easy to work with. After it dried the polish popped off one nail. Is this normal for HT? </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b6so0i/so_many_people_seem_to_love_holo_taco_i_bought_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1b6sg48</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>ILNP's "The Message"</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fy6ihles3fmc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1b6s3e3</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Five coats, what is this, a topper??</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxsmg83z0fmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1b6rhk4</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Break room nails!🧂love this combo, even with the Seche shrinkage..🥲</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1f8rj809wemc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1b6qrnj</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Which one should I choose?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4s9ie3tqemc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1b6ps7e</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Looks like they are addressing the issue with Wolfsbane Encore!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ps7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1b6plp8</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Green so vibrant, it glows a little 🍀</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agu22x45iemc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1b6piih</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Surprisingly Pretty</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0fuwjnihemc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1b6oshm</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>"High Quality Nudis" - Dam Nail Polish (PPU February '24)</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6oshm</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1b6ohi2</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>obsessed with the iridescence</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ohi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1b6nz5x</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No videos? </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pu2feklr6emc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1b6nvvl</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>What is happening to my nail?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbjqy5c66emc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1b6ne9g</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Looks like a reflection of a sunset on water 🌅</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ne9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1b6ncjl</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Mooncat - A Very Merry Unbirthday 💜</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewhxkt9d2emc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1b6nbt6</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Never fail to match </t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhm6vtk72emc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1b6naei</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Gloomy weather requires a shocking pink mani</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3b3vr9bx1emc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1b6n5me</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Air purifier for nail polish odor</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b6n5me/air_purifier_for_nail_polish_odor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1b6n2p9</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting Nails and Making Friends </t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8v0d8fzd0emc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1b6maxb</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Fairy shimmer</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6maxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1b6maut</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>First attempt at magnetic tips</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9ial9suudmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1b6lu1c</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Layered skittles</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddfj83phrdmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1b6kn1z</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>All I Do Here is Ask Questions 🤣</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b6kn1z/all_i_do_here_is_ask_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1b6kdr2</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>First thermal mani</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6kdr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1b6jwjm</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Any Horror fans??</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6jwjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1b6juub</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>ILNP 💙</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0rj0p7bddmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1b6j4lj</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>My sister, me and my friends painted our nails (Twas my friends first time doing so)</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkxegcd18dmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1b6ix47</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Finally, my perfect red magnetic Mani 💅🏻</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ix47</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1b6iqnm</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Can’t get enough of this mani.</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6iqnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1b6gido</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>ILNP Snowstorm</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6gido</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1b6ij90</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Do my nails look neutral or light pink?</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdo63xtt3dmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1b6igj7</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A nice little palate cleanser </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yez80xaa3dmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1b6idn9</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>MC Serpents tongue HT Alien infatuation</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e52e9gsp2dmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1b6hr6m</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>rose quartz nails ✨</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6hr6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1b6hplk</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>TV Girl themed nails</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6hplk</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1b6fucd</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>First time with a thermal and with PPU</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6fucd</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1b6fyo2</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>💨🔥The Avatar🪨🌊</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6fyo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1b6fa9h</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>I must not fear. Fear is the mani killer.</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6fa9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1b6eub1</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>The Color Dept in Avoguac</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i77bi3o0ecmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1b6e8nm</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Building a new stash</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b6e8nm/building_a_new_stash/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1b6e38l</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>1st of a Month of Green March Manis</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6e38l</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1b6dti9</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>If I’m going to be at the beach for a week, what kind of overlay should I get on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b6dti9/if_im_going_to_be_at_the_beach_for_a_week_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1b6cszs</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>OPI - Virgoals</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6cszs</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1b6butu</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Jade</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n0vageasbmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1b6bpxo</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>tortoiseshell nails: first attempt</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6bpxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1b6b9ps</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>A fun springy green from my untrieds drawer! 🌷</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2q9zhd8mnbmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1b6ah5h</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>LynB Chocolate question</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6ah5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1b6a8bo</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Comparison?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b6a8bo/comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1b699um</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>My little '90s collection</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b699um</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1b688or</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b688or/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1b6xpl8</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Just did this set last week. Cc is welcome</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee5eccmfdgmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1b6oin8</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>This is my job</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1b6oin8/this_is_my_job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1b6m7br</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Smoke effect with green. I want to know who loves green like me 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkhm62j4udmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1b6l71n</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Cinnamonroll nails 🩵</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b6l71n</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1b6apfq</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Vintage St Patty's day nails</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r775iccpibmc1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar  6 08:08:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_10.xlsx
+++ b/data/2024_03_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C447"/>
+  <dimension ref="A1:C588"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8032,6 +8032,2403 @@
         </is>
       </c>
     </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1b7u1fx</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Black nails with a twist ✨</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nbpty9af4omc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1b7u09m</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Shaped my square nails into almond? Round? Either way I love them! This is the longest my natural nails have been! Color is OPI’S bubble bath 💕🤍</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltse6ni24omc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1b7tynd</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Semi cured gel nail strips you can recommend?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7tynd/semi_cured_gel_nail_strips_you_can_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1b7tydh</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>My nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uirlyze3omc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1b7s9rq</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Got these done as a Bridesmaid</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa8qsez1lnmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1b7s73y</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Considering offering Russian mani’s!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7s73y</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1b7rq9k</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>feeling blue 💙</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2dwyl5sfnmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1b7rdh8</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Some Sets I've Done</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7rdh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1b7q1m8</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Some sets I’ve done &amp; their names 💖💅🏽</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7q1m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1b7no5v</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>I want to get a manicure, but 2 of my nails are breaking— what are my options?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7no5v/i_want_to_get_a_manicure_but_2_of_my_nails_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1b7m6wv</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>What do you think ?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ljq7jezw3mmc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1b7qnnz</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Rate my nails, looking for honest feedback</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh75m1er5nmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1b7qhzn</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l35ctpza4nmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1b7q2vm</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>V day (late)</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a49bmvpg0nmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1b7py8p</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to strengthen my nails </t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7py8p/how_to_strengthen_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1b7pxmm</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t take care of them in any way should I cut them or something </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12os1c24zmmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1b7px9v</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Can you tell I got a manicure by looking at my hands?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7fv3db1zmmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1b7p23q</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>I have marks on my thumb nails from (I believe) improper removal of press ons and from them being too long and pulling at the nail bed.</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7p23q</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1b7oy07</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Mirror Cat Eye 💅</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ln9az71kqmmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1b7olm1</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>First time trying chrome out and I am obsessed!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oe2cnropnmmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1b7nud4</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>My 90’s-Patty’s Day nails</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uurbh3hhmmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1b7mf33</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t xml:space="preserve">St. Patty's Day Nails.  </t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/baydpcsq5mmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1b7m0zq</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally committed to growing out my nails! </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wofdnkm2mmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1b7hdxq</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>can't get my sets to last more than 2 days, help!!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7hdxq/cant_get_my_sets_to_last_more_than_2_days_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1b7fxtg</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Swimming with press on nails - yay or nay?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7fxtg/swimming_with_press_on_nails_yay_or_nay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1b7k88w</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Decide to add a bit of gold to the wine 🍷 ⭐️</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7k88w</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1b7k4rp</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Cinnamoroll set for my recent trip to Japan 🩵</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7k4rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1b7jtv9</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Do polygel nails last and are they good?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7jtv9/do_polygel_nails_last_and_are_they_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1b7jtr0</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Sleeve over hands in pics</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7jtr0/sleeve_over_hands_in_pics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1b7jdst</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Spring 🌸</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqn9svbgilmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1b7j0xe</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>help needed</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7j0xe/help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1b7ispu</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Black nailsss</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn843k6delmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1b7ihnk</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>What shape nails?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfi9ky67clmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1b7i5so</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>I usually go for edgy but I was feeling feminine this time 🥰</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djl8jr5w9lmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1b7hokf</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>My march set</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7hokf</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1b7hak9</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>So this is my first time trying 3D press on nails</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7hak9</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1b7gljn</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>First time gel extensions at home 🥰</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/258b5axyykmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1b7gbvw</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Tried on some nail stickers (-:</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7gbvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1b7g5i2</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Barbie french? I did to go to Vegas - too much for spring?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad16qigyvkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1b7g0tm</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>First time at nail salon help!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7g0tm/first_time_at_nail_salon_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1b7feo2</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>got mine done for the first time!!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2wkp2tnqkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1b7f9zg</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>🍓🍒</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnczubrrpkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1b7ebdj</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Do these nails look bad? Don't know much about nails.</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7ebdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1b7ez6e</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>OMG 😍😍</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z660237nnkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1b7eylk</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something different for a change </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lddysxjnkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1b7exzt</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Anyone know where I could find these Beauty Avenue Raw Gel Nail Seal or any similar products in the US of Canada?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7exzt/anyone_know_where_i_could_find_these_beauty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1b7ewcg</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Coraline nails 🖤💙</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44wf1e06nkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1b7em6h</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Which nail shape is best on me?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7em6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1b7e7sr</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Glowy orange 🧡</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmi08kddikmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1b7dyy7</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Latest obsession is mix matching colors ❤️🩷</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7dyy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1b7d7nn</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>When you want nice nails but your fingers look like this, what you doing mate I ain't no carpenter</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7d7nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1b7cpmw</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Why do my finger nails look like this?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7cpmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1b7bauu</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>How do you wash your hair with press-on nails?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7bauu/how_do_you_wash_your_hair_with_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1b7cjzn</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Felt cute, won't delete later ^^</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpjvxipt6kmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1b7ch5t</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Russian Nails on Long Island (Nassau county)</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7ch5t/russian_nails_on_long_island_nassau_county/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1b7bnbt</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Neon croc nails</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wimqox4i0kmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1b7bb76</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Should I change my nail shape?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xac2rml6yjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1b7b07f</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>For all the TrueCrime/80s fans out there</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7b07f</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1b7a1b9</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Set from last summer, I love my tech 💕</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9slavvapjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1b79tjv</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Gel nails suddenly always chip?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b79tjv/gel_nails_suddenly_always_chip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1b79liy</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>YAWL I HAVE A QUESTION</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b79liy/yawl_i_have_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1b77g6w</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>First time doing square</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlj641867jmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1b76cfr</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Gloves in shower</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b76cfr/gloves_in_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1b791gg</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>I never get sick of holos 🌈✨</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2rputeeijmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1b78uhw</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b78uhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1b78s8v</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>My birthday present🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkifmemogjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1b78ba9</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Are there any fans of this cartoon yet?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh2tabkfdjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1b77ywz</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Wear ring to appointment?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b77ywz/wear_ring_to_appointment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1b77r32</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Bold or subtle accent nails?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b77r32</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1b77lwy</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>pla be honest should i get this fixed?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b77lwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1b761ck</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Just playing around with silver leaf foil 😇 love the idea, but I hate that I have so shaky hands 😅</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcnicn39wimc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1b71enu</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Freshly painted 💅🏻</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lvhzfmpkhmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1b70x4k</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just a little moonstone </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asht9eofehmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1b70jzd</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Nail Extensions on my Grandma?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b70jzd/nail_extensions_on_my_grandma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1b70awc</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>just got done today!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b70awc</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1b7u5sj</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Ignoring the odd shooting star colours, I’m now in love with the idea of a planet set</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7u5sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1b7tm9t</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Fragrance oil in cuticle oil</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7tm9t/fragrance_oil_in_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1b7sk7m</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner looking for products to speed up dry times and longevity </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7sk7m/beginner_looking_for_products_to_speed_up_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1b7s2mj</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Mooncat - Weeping Willow</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7s2mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1b7rw9x</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Adriana girl cmon</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9n2961ehnmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1b7rqcn</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Broke a nail, decided to try a cheap purple I’ve never done before while I grow out!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7rqcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1b7qqi0</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Any Lacqueristas who are artists?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7qqi0/any_lacqueristas_who_are_artists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1b7q7lc</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>fake halo</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7q7lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1b7peed</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Polish after top coat</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7peed/polish_after_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1b7p8fy</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Spring has sprung</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7p8fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1b7p26c</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Getting ready for St. Patty's Day like...</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2gglxuirmmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1b7o091</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>I have to limit how much I wear pink because it will make me stare at my left hand allllll the time</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fj548h0uimmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1b7mb6f</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Best stamping I’ve done so far!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7mb6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1b7l5ht</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Zoya-Tamiah</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ac47a8ovlmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1b7k3jb</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Redo with creme base</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7k3jb</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1b7jjxi</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Coworker asked me if they were fake 💅</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7jjxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1b7ivdk</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>First time poster in this sub!! Loving the length I've got right now, as well as this fun polish!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7ivdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1b7iu3p</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Shape?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjp8im2nelmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1b7ia70</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Do I need this??</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9sv9meralmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1b7i7pi</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>I don't see a lot of love for Emily De Molly, but their polishes SLAP!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/huvoli29almc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1b7i5fy</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Monophase builder gel and lifting</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7i5fy/monophase_builder_gel_and_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1b7h22n</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Pink to green duo/multichrome?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7h22n/pink_to_green_duomultichrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1b7fy7o</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>february’s nails (see them grow)</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7fy7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1b7fqqm</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Bisou Bisou perfectly matches my desk set up as long as I’m not too cold</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7fqqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1b7ewfb</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Bit disappointed</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7ewfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1b7er79</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Prism Polish ‘The Silence’ 💿</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa33atx5mkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1b7eka1</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Bearly Frio sub</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45ck8cmokkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1b7eg6e</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>And just like that, St. Paddy's Day in my tips...</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssto279zjkmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1b7ea6d</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>february nails 💝</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7ea6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1b7e9fp</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Just convinced myself I need more polishes with this mani</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7e9fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1b7difv</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>My polish always peels off in one piece.</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4nftnkfdkmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1b7dgnu</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Unique polish- Toxic Sludge</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7dgnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1b7cs50</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>A Love Poem I Used to Know</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7cs50</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1b7cqvy</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Playgirl 'Finland'</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/s9Ls5ED</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1b7c73z</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>HEMA in Olive and June??</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7c73z/hema_in_olive_and_june/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1b7b1np</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>FYI,the Target Dollar Spot has coffee pod drawers and tissue boxes that work WONDERFULLY for storing nail supplies.</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7b1np</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1b7av3e</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Lyn B Designs - Kitten Purrs</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/76agrkezujmc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1b7alar</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>My best attempt yet</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vjrebj3tjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1b7acnl</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Heard it was Women’s History Month</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crr0v4igrjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1b7a6q8</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Question about Ethereal drops</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b7a6q8/question_about_ethereal_drops/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1b7a6cr</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>ITS CORN</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7a6cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1b798qo</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Are mediocre manis with crusty cuticles accepted here?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk4sbr1tjjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1b79084</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Getting in the March mood - ILNP Bottoms Up</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b79084</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1b78wom</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>holo and shimmer are my whole life I think</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b78wom</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1b78o0n</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>ILNP Dakota</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b78o0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1b78kit</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>normal wear &amp; tear for Cirque jellies? 3 day wear</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b78kit</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1b78i4a</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍳 Now I just need to learn how to do bacon 🥓 </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4ex37krejmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1b78csz</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo there, lacqueristas!✨ </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0h7ad4qdjmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1b77wd0</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Builder gel question - do I need to buff the builder gel before applying the gel color?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b77wd0/builder_gel_question_do_i_need_to_buff_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1b77cms</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Rainy day Penelope Luz- Hush, hush</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b77cms</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1b769kd</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Gloves during shower</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b769kd/gloves_during_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1b75tgg</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>kur by Londontown Illuminating Nail Concealer Trio at Costco</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sa7yxrzkuimc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1b74c1q</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Lacquergram daily</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b74c1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1b741i8</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Guess who bought a dotting tool</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkpdn3hoeimc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1b73sn5</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Obsessed.</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0cey85o5cimc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1b70w2v</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Sassy Sauce LSD</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d0rhrsizdhmc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1b70ja7</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>First flower for attempt!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b70ja7</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1b7ouim</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Lunar New Year nails</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7ouim</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1b7n28j</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>First time DIY Acrylic set</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7n28j</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1b7m1uk</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Finally committed to growing out my nails!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxvjanft2mmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1b7jv3p</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Creepy cute</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ug3au2bvllmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1b7jsk0</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Slim oval with some stone and caviar design. I love to apply multiple size stones and make minimalists designs! What do you think? 🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7jsk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1b7inai</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>I made a minimalist design❤️ what do you think? 🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3c71vcbdlmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1b7ckl7</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Loteria Nail Art</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3uvmv2y6kmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1b77tym</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>The simpsons treehouse of horror nail design</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b77tym</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1b75lsi</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Ocean nails</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b75lsi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar  7 08:04:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_10.xlsx
+++ b/data/2024_03_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C588"/>
+  <dimension ref="A1:C711"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10429,6 +10429,2097 @@
         </is>
       </c>
     </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1b8oupw</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Some simple nude nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8oupw</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1b8ogto</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Have your gelx nails popped off while the actual gel stayed on?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74n25sex4vmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1b8mdi3</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Hard, dry skin around nails. Help!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8mdi3/hard_dry_skin_around_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1b8lg9r</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Glazed Daises?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8lg9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1b8l1nr</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Encanto Inspired </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59uuollh7umc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1b8j9ee</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Silk wraps for split nail?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8j9ee/silk_wraps_for_split_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1b8i991</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Not sure if right sub, but need advice on next glue on</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8i991</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1b8hypb</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Why does this keep happening? (3/10 nails currently like this)</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkvrswlshtmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1b8dc0j</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Is this normal for gel top coat?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8dc0j/is_this_normal_for_gel_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1b8l5vd</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Press on recommendations/ alternatives</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00yczcij8umc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1b8l1ux</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Curve nail question</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8l1ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1b88jr2</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Need some advice to take care of my nails</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b88jr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1b8kgu1</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>An uncle on a mission. I did my nieces nails for the first time since she had her baby.</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xxa03cg2umc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1b8kcr3</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>is gel better for dry skin?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8kcr3/is_gel_better_for_dry_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1b8jsja</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Jelly Gel Recommendations</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8jsja/jelly_gel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1b8jmbg</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Chonky glitter acrylic ombré for March :)</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8jmbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1b8j2ux</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>shimmery glow in the dark nail polish recs?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8j2ux/shimmery_glow_in_the_dark_nail_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1b8it1m</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>2 of my natural nails snapped off today. Went home and super glued them back on. How’d I do??</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8it1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1b8hwy0</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set for Spring🎀 gel overlay on my real nails </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sm7rgqsehtmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1b8hbhm</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Is it normal for nails to grow this fast?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k02m9cpmctmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1b8h5e5</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Why do some of my nails have push-ins like this?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8h5e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1b8h4d5</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>gel overlay on my real nails :)))</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8h4d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1b8h0ub</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Berenstain Bears 🐻</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8h0ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1b8gh66</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Totoro nails!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0e2qnfiw5tmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1b8fyl0</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Chocolate with some frost: yea or nay?🍫❄️</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8fyl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1b8fwtw</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>So proud of my girl!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8fwtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1b8ex4h</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Cheerful</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72cqch9utsmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1b8euia</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Cute black and white nails 🖤 🤍</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6huq710btsmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1b8emte</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>It's my 29th birthday so I made some nails to celebrate! Everything is hand sculpted and hand painted.</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8emte</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1b8dya1</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>(First post🙈) Did my own French tips with BIABx</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4s59wlzmsmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1b8dapv</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Using builder gel to attach tips?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8dapv/using_builder_gel_to_attach_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1b8cvv2</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Spring is near 🌿</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ioeoynifsmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1b8byhp</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Love my nail artist</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvy2mlkv8smc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1b8bmw6</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>😭 what should I do? Cracked my nail reaching for my phone in my pocket</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ikpwh1n6smc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1b8bf3i</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>🐮</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ldex4235smc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1b8b8nd</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Easiest method for beginners?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8b8nd/easiest_method_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1b8b835</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Honest opinions?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkdzvaso3smc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1b8b0kx</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Baby pink chrome</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8b0kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1b895n3</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Palate cleanser...but make them ✨fancy✨</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b895n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1b8945f</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>First attempt at DIY custom press-ons. Suggestions on how to improve?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8945f</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1b88qi4</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>October Vs March</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b88qi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1b88a7e</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Are you into spicy nails? I tried a new style! Thoughts? 🤍 _(´ཀ`」∠)_</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b88a7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1b86utz</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Is it that bad?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b86utz</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1b86pw9</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Lavender nails🪻</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5xgcask8rmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1b8699j</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Buffing/texture for gel nails</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8699j</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1b866lr</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Natural nails super weak</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b866lr/natural_nails_super_weak/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1b85ndb</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>French Mani</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b85ndb</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1b84va9</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Beautiful ombre with glitter!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b84va9/beautiful_ombre_with_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1b846fp</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Made these myself for "Fat Thursday" occasion</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bpkuwqerqmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1b81fw3</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French mani for an anxious person with short, thin nails. </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b81fw3/french_mani_for_an_anxious_person_with_short_thin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1b80cs9</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fake nails fall off next day in the shower help! </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b80cs9/my_fake_nails_fall_off_next_day_in_the_shower_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1b838mz</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Idk how I feel about them, thoughts?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b838mz</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1b83271</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>glazed donut nails 🩰🪽</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b83271</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1b830jn</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Has this happened to you?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b830jn/has_this_happened_to_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1b82yne</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>New mani</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44bz85nxiqmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1b82pmq</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Got my acrylics removed!</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b82pmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1b82kfe</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hacks for broken nails ? </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b82kfe/hacks_for_broken_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1b828tn</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails with bffie </t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mpvrc1pdqmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1b81vx5</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>How to make press on nails last a shorter amount of time</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b81vx5/how_to_make_press_on_nails_last_a_shorter_amount/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1b7zui6</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Should I invest in press ons? Should I invest in buying professional materials and do my nails at home?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7zui6/should_i_invest_in_press_ons_should_i_invest_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1b7zalm</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>How many dips per nail?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b7zalm/how_many_dips_per_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1b7z33h</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7z33h</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1b7z19c</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>What nail length and shape look best on me?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7z19c</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1b7yp4u</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Shout out to my nail tech 🫧🌸</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9eorotuklpmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1b7xltw</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Chess nails made by me ♟️</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7xltw</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1b8lhjh</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Brite is Nice</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhcujldhbumc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1b8knhg</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Little evil eye</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8roeng24umc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1b8kkng</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Blurple multichrome</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8kkng</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1b8k2wp</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>So many purples in just one polish!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8k2wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1b8jras</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Dune Nails!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8jras</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1b8irdh</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Spring polish for those of us with red hands/reynauds</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b8irdh/spring_polish_for_those_of_us_with_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1b8i5il</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>This is Mermaid Bait by Mooncat. My first Mooncat polish and lacquer polish. Absolutely beautiful 🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8i5il</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1b8i4qs</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>I'm craving caramel</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8i4qs</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1b8i4a2</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color Order Options for Organizing Collection </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b8i4a2/color_order_options_for_organizing_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1b8hebh</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A pop star purple moment </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cljr6u09dtmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1b8gzg2</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Pisces season inspired nails ft Gracie</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8gzg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1b8gt5q</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Flower Power 🌸💜</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8gt5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1b8go2s</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Got these press-ons from a new Swedish company and love them so far 🥰</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilgt9prf7tmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1b8gn6q</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Easter egg nails</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8gn6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1b8bakw</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Regular Polish and Chrome Powder</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8bakw</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1b8fpif</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Been a minute since I did a new mani.</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm1ywaevzsmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1b8en1k</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Lil Lizard 🦎</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8en1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1b8dr73</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>When you can't decide which color</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8dr73</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1b8dcyg</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Looking for a chocolate brown nail polish</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b8dcyg/looking_for_a_chocolate_brown_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1b8dc04</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>It only took me 4 days to capture this thermal at the right time 😂</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4fgvv1mismc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1b8bnnd</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Anyone heard of this brand?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khcnda7s6smc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1b8bf8g</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>first time using magnetic gel polishes</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux4j9x445smc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1b8aemz</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Ethereal - Now Go and Don’t Look Back</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mxcnrzmxxrmc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1b8a16s</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>⚡️🖤Black Ranger🖤⚡️</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8a16s</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1b89wt2</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Matte finish short nails</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b89wt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1b89a7w</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Looks like childhood! 💕🦋</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b89a7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1b87owl</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Beginner nails</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kngp9805frmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1b87ngg</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Looking to add to my collection</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b87ngg/looking_to_add_to_my_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1b87l79</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Trouble magnetizing Mooncat’s ‘Velvet Rose’?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b87l79/trouble_magnetizing_mooncats_velvet_rose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1b87hvh</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Manicure after five days! Now to decide what color(s) to do next 😅</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfw9wprsdrmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1b86u5w</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>What makes a professional gel polish🤔</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b86u5w/what_makes_a_professional_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1b86q2n</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Nail oil was an absolute game changer</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b86q2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1b86at7</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Spirit Fingers &amp; some comparisons</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b86at7</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1b85hat</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Cirque zeitgeist + Kathleen &amp; Co. toasted marshmallow ☕</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b85hat</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1b85eif</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Industrial magnets are a game changer</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b85eif</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1b84t1y</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>I swear my shower just makes all of my polishes 10x more gorgeous</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6g4euqbrvqmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1b84a6s</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Looking for the most purple of purples that ever did purple</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b84a6s/looking_for_the_most_purple_of_purples_that_ever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1b83im2</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Boolba over Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9tgsdjrmqmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1b83a0y</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>glazed donut nails 🩰🪽</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b83a0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1b82tkh</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I want it so bad, but it's so similar to something I already own. Help!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b82tkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1b81vkm</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>How to make press on nails last a shorter amount of time</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b81vkm/how_to_make_press_on_nails_last_a_shorter_amount/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1b81s49</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>My mid-week color refresh</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b81s49</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1b80jqt</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Not perfect, but I love the colors.</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4j6g6y21qmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1b801zq</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>I made my own fruit themed nail stickers!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b801zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1b7w5hu</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Both my thumbs do this ): How can I stop it/take better care of my nails?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7a4dpcduomc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1b7upfk</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>The ✨GLOW✨</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b7upfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1b8l37r</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Encanto Inspired </t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkrsrz8v7umc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1b8h1ec</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Berenstain Bears 🐻</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8h1ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1b8cu4f</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>saw this on painting pinterest and had to try it on a nail</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8cu4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1b8c4b0</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>checkerboard is harder than it looks</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckff8lk1asmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1b8905s</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>These are called ballerina nails. I made a colored babyboomer and put some holographic glitter to the cuticle area. What do you think?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8905s</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1b87k55</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Love this colorful design</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b87k55</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1b84zsq</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>beginner nail artist—recent sets!</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b84zsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1b84ymm</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Bulbasaur</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b84ymm</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1b84hg3</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Newest sets</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b84hg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1b83hgr</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Pretty happy with my latest graphic mani! First time trying checkerboard on myself!</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b83hgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1b81u8z</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Arched square and a black French with some animal prints design at the cuticle. This design can be made with any color. What do you think? ❤️‍🔥🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b81u8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1b7zmrb</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Sometimes you have to accessorize</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8cfpp8otpmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar  8 08:07:31 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_10.xlsx
+++ b/data/2024_03_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C711"/>
+  <dimension ref="A1:C848"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12520,6 +12520,2335 @@
         </is>
       </c>
     </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1b94x3g</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Help- how do I keep my nails from breaking like this?? The break always starts on the nail bed</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b94x3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1b92h54</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Structured gel</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5phtr7gflymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1b90mii</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>white spots on polish?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mwizd588ymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1b8xcxv</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>How to keep from flaking off during martial arts?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8xcxv/how_to_keep_from_flaking_off_during_martial_arts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1b8v0qm</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Inspo was marble but I ended up with kitchen countertop</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8v0qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1b8r0g8</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Awful natural nails</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8r0g8/awful_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1b9hgty</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Tried to file these down from square to coffin and I think I did a pretty good job 🥰</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhzhzrnb22nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1b9hbr1</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>I am in a nail biting cycle and I am looking for THE solution! Help!!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b9hbr1/i_am_in_a_nail_biting_cycle_and_i_am_looking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1b9garm</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>First time trying nail art!!</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvaqemplq1nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1b9fwpa</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>240 grit good quality glass file recommendations?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b9fwpa/240_grit_good_quality_glass_file_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1b9fnyf</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Finished painting my princess &amp; the Frog (Mother's day edition) nails 💗</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/57136vrrk1nc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1b9f8do</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Weekly Polish Change</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofpji9sqg1nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1b9eujj</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I’ve been wanting rainbow nails for a while now! I went to get them done today</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9eujj</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1b9e1s4</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dip powder nails. What’s going on with my pinky nail? </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uucis33c61nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1b9dtrb</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>I love a good short set once in a while</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqxffkcf41nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1b9dscb</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>nail press ons help!!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t2dulf341nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1b9dpgq</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>My lovely nails</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9dpgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1b9dkqk</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>I am obsessed! 🫶</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9dkqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1b9dcfj</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Does this tip look better on coffin?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7enx6nd01nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1b9d8ij</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Just did my nails! 💅</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9d8ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1b9czqa</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Does this nude color compliment my skin?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4jaa4cfx0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1b9ct4r</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Red red reddd</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g0xx5zuv0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1b9cqzd</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Did my sisters nails!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e3b085dv0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1b9bwb8</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Spring-ish</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sabz4ledo0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1b9brr7</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>My first time trying pop art nails, went great!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9brr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1b9bqlg</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>FROGGY</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9bqlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1b9bgxm</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>St. Paddy’s Nails</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9bgxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1b9basz</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>An oldie but a goodie💫</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzxx9sohj0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1b9babr</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>New press on‘s &lt;3</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9babr</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1b9b7l2</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Lucky Charms nails for March! 🍀</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejddimtri0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1b9aleg</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Favorite shape for strength?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b9aleg/favorite_shape_for_strength/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1b9a7h8</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Are my nail beds that good?…</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/raoat6rra0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1b99mbv</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Gel-X for the first time</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b99mbv/gelx_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1b98eou</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Do you know what color this is?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3hb9kqeuzmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1b97oik</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Are press ons allowed? I’m still a beginner but very proud of how this set came out 🥰</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k90cvccxozmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1b97gp8</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Chrome ombré 🪩</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b97gp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1b977wd</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Hatsune Miku nails!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgbj6tcmlzmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1b965bk</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to shorten nails </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b965bk/how_to_shorten_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1b95zhf</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Any water permeable nail hardeners out there?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b95zhf/any_water_permeable_nail_hardeners_out_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1b95pk8</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Rainbow for spring 🌈</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utdv1byyazmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1b95f9t</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>new nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b95f9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1b94w7k</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Simple Russian mani!</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfhrxj775zmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1b94o1y</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Where to get embellishments?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b94o1y/where_to_get_embellishments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1b94h30</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Saint Patrick’s day vibes 🍀</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9evrkwc62zmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1b94fxo</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Rosy Transparent Nails 💕</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b94fxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1b94fba</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Colorful sparkly nails 🥳</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b94fba</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1b93uvg</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Puppy theme nails 🐶💅</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b93uvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1b93sdc</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Lollipop set -part 1</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b93sdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1b93fhe</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New rainbow nails </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sp01tm1xuymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1b92ndg</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Longest nails I’ve had so far</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aat23ocxmymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1b92awe</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>I was called "delightfully fancy" when a friend saw my most recent design.</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/183ktzt4kymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1b929qt</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My recent sets 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b929qt</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1b91kqq</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Glazed donut structured gel Russian mani….my new nail tech KILLEDDDD</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lmp52sueymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1b91e5h</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>St. Patty’s came a little early</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b91e5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1b91a88</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>In love💕</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpriwwatcymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1b911l3</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>My current nails done by my cousin</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/za7qz9s5bymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1b90z73</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Having fun with nail art:)</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ob5cwxnaymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1b90yfj</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Back again with more marble nails:)</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33t8g95jaymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1b90x96</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Rawr💖💕💗💓</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hskje7cbaymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1b90wms</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I’m obsessed with marble nails😍</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b90wms</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1b90q0r</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Black, White &amp; Chrome 🖤🤍🩶</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b90q0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1b90p2v</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Spring Drip</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7l15hflp8ymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1b902ct</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This has been my favorite combo this winter </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lp1p9x9c4ymc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1b8zn9g</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>First time used stamps</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apuheqrd1ymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1b8zduu</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>What do you think</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8zduu</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1b8y9e3</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Newest set! I wanted green for March but couldn't pass on this pretty color!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8y9e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1b8wvin</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Help with brittle nails</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io5itfyegxmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1b8wprc</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Got a new job and wanted to celebrate with lots of colors!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8wprc</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1b8w8w1</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Springtime</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4df1kwmqbxmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1b8vn73</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>💛💚💙💜🩷</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pk55ru127xmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1b8sy2d</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Gel nails and extensions</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i0kualkjwmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1b8soax</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>I made myself this ballerina nails with a very smooth babyboomer and applied some holographic effect at the cuticle. What do you think? ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8soax</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1b8saq3</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Arched square with some animal print design and black French! This design can be made with any color and any animal print designs. I made this manicure for a person that have really big problems with her cuticle skin area. What do you think?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8saq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1b8rqk5</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>I love my simple new bubblegum gel polish 💗</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apfgsoyq6wmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1b8r4yp</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>first time getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8r4yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1b8qwgs</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>First time using reusable tips</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8qwgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1b8q975</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a thick  “gel like” nail glue that doesn’t require UV lamp . </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8q975/looking_for_a_thick_gel_like_nail_glue_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1b8q5y8</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Should you take a break from sns every now and then?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b8q5y8/should_you_take_a_break_from_sns_every_now_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1b8pnqw</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting a princess &amp; the frog nail set (mother's day edition) 😍 </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u8sc2k68ivmc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1b9iuft</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Sorry for the jump scare, what colour would look good on my poorly circulated feet?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gly6ktph2nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1b9g510</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Favorite pastel green polish?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b9g510/favorite_pastel_green_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1b9fyq8</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Pink glow is so hard to find but when you do (ﾉ◕ヮ◕)ﾉ*:･ﾟ✧</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4kzod52gn1nc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1b9fopj</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>[help!!] did my nails slightly rip off the nail beds?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9fopj</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1b9cz14</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Jumping on the green wagon 🍀</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hy3mh1z8x0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1b9avlb</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Basic white</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hduq4us2g0nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1b99upw</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Hummingbird - Penelope Luz</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b99upw</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1b98ujl</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Need a polish similar</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b98ujl</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1b98l9y</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>florals for spring? groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b98l9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1b98ccn</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Best my nails have ever looked</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdf6iqottzmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1b988yc</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Velvet effect with Starrily's Serpent's Lair</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b988yc</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1b988s8</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Cirque - Introverde</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b988s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1b975bi</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Make it blue! Make it pink!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b975bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1b9739k</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>ILNP ASAP</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgn0kq5okzmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1b96dbh</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>How would you pack this for a cross country move?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b96dbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1b960lo</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Mooncat Midnight Rider (my cat is a paid extra)</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2m3jcx4dzmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1b95vrr</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Daveen Lacquer has stole my heart!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b95vrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1b95poq</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Best Golds?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b95poq/best_golds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1b95h59</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>First ever thermal, this may be my new addiction!</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b95h59</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1b95cd0</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Arsenic on the Rocks</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/udyvk80c8zmc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1b95azf</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>A classic red while I wait for spring</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b95azf</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1b944hd</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>🪩✨🌈</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b944hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1b943h4</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Mid flight nails 🛩️</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b943h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1b93m3r</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Rainbow Roar</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlomqj29wymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1b92jiz</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Is stamping polish good for nail art?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b92jiz/is_stamping_polish_good_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1b928na</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>nitrile gloves have ruined my nails - lab workers, any advice?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b928na</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1b924xz</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Any dupes for OPIs Got The Blues For Red?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7g0s0uwiymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1b91q7d</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Shrooms</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm67tfmxfymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1b91eqb</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Silver Counts As Neutral, right?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b91eqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1b91e5e</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Fun with Eclipse</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b91e5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1b91axz</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>sparkle city</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b91axz</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1b910wu</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Retro Teal 🏖️</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b910wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1b90iap</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>One coat of sugar daddy and one coat of good to go top coat for the ultimate sheer pink look 🫧</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jf7r0xe7ymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1b8zzlf</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Nail Glue</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g06vm5ys3ymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1b8zzdr</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Good lighting at the river!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8zzdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1b8zvln</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>🍀🍀🍀</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8zvln</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1b8zt53</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frozen fingers but shiny nails </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oyp68rsi2ymc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1b8zeaz</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Your favorite pink creme nail polishes</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b8zeaz/your_favorite_pink_creme_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1b8zbpz</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Starsword</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjc9np64zxmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1b8z3ql</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Glowy Springy Green</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8z3ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1b8z3ax</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Been growing out my nails for over a month!</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ftxlxkhxxmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1b8yyg4</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Help with dark marble?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8yyg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1b8ycgq</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Second attempt polygel over natural nails</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8ycgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1b8ua3r</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>My first Mooncat 🌙 🐈‍⬛ and I’m in love!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8ua3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1b8td69</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Any dupe recommendations for this shiny green polish?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efone04lnwmc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1b8sxun</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Light Blurple</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/99hqehw</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1b8scax</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Shaping struggles</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyl6mp07dwmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1b9fphz</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Finished painting my princess &amp; the Frog (Mother's day edition) nails 💗</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2qrcu7a5l1nc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1b9dxh1</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Out in Space</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9dxh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1b9dgep</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Gel nails✨💅</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lowij5ka11nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1b9768w</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Hatsune Miku set I just finished!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9n3m4w9lzmc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1b93pln</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Lollipops set -part 1</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b93pln</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1b93n2c</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Natural square with some degradé (fade) made in the no file technique. Size 4 on the template, combi manicure. For the bonus I made a stones design. What do you think?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b93n2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1b910u1</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Obsessed with red marble nails:)</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b910u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1b90pt2</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Spring Drip</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ls9cf8ru8ymc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1b8zxop</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>first spring nails of the year🌸</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6q7pi80f3ymc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1b8v39l</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>My 1st spring set 🌸🍃</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b8v39l</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1b8pnbr</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting a princess &amp; the frog nail set (mother's day edition) 😍 </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3domebd3ivmc1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar  9 08:06:45 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_10.xlsx
+++ b/data/2024_03_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C848"/>
+  <dimension ref="A1:C971"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14849,6 +14849,2097 @@
         </is>
       </c>
     </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1bacfyr</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My grandma loves it when my nails have design, so I made this extra special in preparation to see her :) </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b4gd4r8k9nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1bab2wf</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>First time getting nails :)</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axr5ek2n49nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1baavco</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Proud in purple</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynj5ocdk29nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1baarf7</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>I love nails 😍</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bavgm9mg19nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1baa6b7</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>How is my press on application?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baa6b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1baa4l5</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>My nail tech keeps using eyeshadow lol</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uysolajev8nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1ba7ztg</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Help me find the perfect nude!!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba7ztg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1ba94xn</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>New March Set 💚</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjsvyjdrl8nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1ba92py</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Lil Bit Irish</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqiz9f16l8nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ba7yp9</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>It’s not spring here in Canada but all the floral nails are giving me fomo. Here’s me trying to manifest it</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba7yp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1ba7u7x</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Spring pastel nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba7u7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1ba7fk5</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>One of my fav sets 🇬🇧</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjb19t3q58nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1ba6x1x</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>How urgent is this to get filled?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xdqxtq618nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ba6smw</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Vacation nails 🤍</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5n52av108nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1ba5kua</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chocolate swirl nails </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgxtg2slp7nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1ba5k6l</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Feelin' springy!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba5k6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1ba3jnz</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>My tech is the best ❤️</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jie6u1g397nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1ba3cdj</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>New set love</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba3cdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1ba3aor</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Gel X set I did for my best friend!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba3aor</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ba2m0i</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Lucky Charms for St. Paddy’s day 🥹</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba2m0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ba18lx</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>My first acrylic set!!!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba18lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1b9w9q0</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>What to ask for at a salon?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ub8p28m8s5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ba24ci</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Nail shape help</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba24ci</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1ba1dnh</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>My mom’s new set - poly gel overlay and painted flowers</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oamruvwqs6nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ba0k1z</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>One of my favorite sets I’ve had so far, my nail tech did such a good job at bringing my vision to life! Gel manicure done by Bri at The Color Bar in Gardner, MA</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba0k1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1b9zah2</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Friday Night Nails 🪩</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9zah2</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1b9y5fk</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>✨simplistic✨</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9y5fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1b9xivp</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>First time trying Ballerina nails ✨</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w3oy0b616nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1b9xe6v</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>My nail tech is excellent, I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilts62g806nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1b9x4sn</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>I painted galaxy nails!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88uwqq2dy5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1b9w1sk</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Squiggly 〰️</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svrftn5rq5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1b9vogx</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>i adore these press ons! 🖤</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj2mp692o5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1b9v1cl</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Easter Nails</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwwjyppkj5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1b9uqrk</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>How much to tip for 35 dollar shellac?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b9uqrk/how_much_to_tip_for_35_dollar_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1b9ubuo</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Please help! What’s up with my e-file? I need to file my nails right now, but it isn’t working</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/md3t0dene5nc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1b9tt27</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>My cousin did a set on me</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8f4rp32b5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1b9t4tk</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>First set of spring 💜🪻</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hsfhx6b65nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1b9p376</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Best affordable nail art kit + stickers for a beginner?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b9p376/best_affordable_nail_art_kit_stickers_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1b9nllo</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Ridges down middle of nails?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qjsolh414nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1b9rxhs</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>what do you think of this new set</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hw87jxrux4nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1b9qixj</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Late Valentines 💘</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9qixj</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1b9q8hl</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Glue ons</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9q8hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1b9psga</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>St Patty Month Nails</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8v97pdoi4nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1b9p0yh</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo Taco's Full Charge and Gold Play Button are the perfect St. Patty's Day combo </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6oj3kg3xc4nc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1b9okai</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Testing out my BIAB colours</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsfwtskc94nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1b9o31c</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Question about brittle nails</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b9o31c/question_about_brittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1b9o02d</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jn2syujn44nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1b9mpz4</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Biab nails lifting even though I cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1b9mpz4/biab_nails_lifting_even_though_i_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1b9mh52</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>It’s an alien invasion</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/za3hy6uoq3nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1b9mfik</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>basic but i love them</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46ydyt19q3nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1b9lszm</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Eyeshadow for gel polish nail art?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9lszm</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1b9jn7u</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>How often do you get your nails dones?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfqnkcpzq2nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1b9jarq</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I thought I was doing so good and then I cut some produce</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5wpjjsum2nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1b9bvq0</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Bugs!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9bvq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1b95otz</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Please help! I have never experienced this issue before with my cuticles peeling like they are. I have tried lotion, oil, hand masks, changing my hand soap, not wearing polish, etc. Does anyone know why this could be happening? I look down and my fingers are bleeding randomly and I hate it.</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b95otz</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1bab8mc</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Deep blue home gel manicure</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bab8mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1baano7</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Sunrise Trip 683 - Chanel</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baano7</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1baa27y</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Quick dry top coat</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj8v7ndru8nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ba8vpc</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>☁️ DayDream ☁️</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba8vpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ba8s2d</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Love this combo!</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wklqjlnbi8nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ba85e5</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Tried the washable glue hack but one finger nail got wrinkled?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inllb9n9c8nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ba7z6x</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>BKL Gwyn</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ba7z6x/bkl_gwyn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ba7jop</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Pastel spring mix of jellies and cremes!</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba7jop</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ba6yg1</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>My birthday nails</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba6yg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ba6wvu</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Best Base Coat For Nails That Peel?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ba6wvu/best_base_coat_for_nails_that_peel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ba6wop</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skipping paddy’s day and headed right for spring </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3wkzbf318nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ba6sua</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Are my nails too damaged for press ons?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvf1qtq308nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ba6fct</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>EDM Surreal Scene fresh &amp; after 1 week</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba6fct</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ba6d7v</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Green mani for March</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grr90qy9w7nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ba5lmc</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chocolate swirl nails </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzm5fxdsp7nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ba4xuy</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>When there's good lighting</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba4xuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ba4oob</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can anyone compare Cirque’s Rothko Red to Mooncat’s Queen of The Dead? </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ba4oob/can_anyone_compare_cirques_rothko_red_to_mooncats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ba2jg2</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Manifesting spring and flowers 😌</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba2jg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ba2eqf</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these while in a meeting earlier today. </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9evjumf07nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1b9whet</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Best UV gel polish?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b9whet/best_uv_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ba1n7u</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Mooncat - Head in the Clouds, Sand Viper, Your Heart’s a Black Hole</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba1n7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ba1l5z</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>USPS delivered!!! I thought they were permanently stuck in transit</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba1l5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ba1jss</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Mercury’s Tears and Ghosts of Hecate</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba1jss</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ba17xn</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Press F to pay respects 🥲</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qf0w1w4jr6nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ba0nsp</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>ILNP vs Static vs Mooncat</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ba0nsp/ilnp_vs_static_vs_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1b9ztyv</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Swatch of my first thermal nail polish, Once in a Blue Moon by Fancy Gloss. So beautiful and reactive!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/q3sapCI</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1b9zr1j</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Green Nails for St Pats and a question about drying drops!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9zr1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1b9z9jk</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Blurple Multichrome Part 3</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6nckigjld6nc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1b9z4z8</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Blurple multichrome part 2?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9z4z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1b9yzi4</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Gel Top Coat Craters</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bfrasbnb6nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1b9xq0v</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Glazed 2024</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpwwfw8j26nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1b9xfye</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I'm starting to like this contemporary design I made up on the fly</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9xfye</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1b9w2d5</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>🫠Trippy Dippy🫠</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9w2d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1b9vz9o</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Good enough I guess</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz4756g8q5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1b9vbpm</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Help me find the perfect nude!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9vbpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1b9vb2t</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Spring Fun</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9vb2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1b9uzxo</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>It's giving multigrain</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9uzxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1b9uutl</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Best affordable nail art kit + stickers for a beginner?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b9uutl/best_affordable_nail_art_kit_stickers_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1b9uobq</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Obsessed with Emily de Molly Check It! Strongest thermal I’ve tried, and so glowy!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9uobq</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1b9udkh</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Accidentally bought a jelly</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9udkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1b9u28c</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Glass Jellyfish</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxk2rcwpc5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1b9u0ia</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>How do y'all have patience for magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b9u0ia/how_do_yall_have_patience_for_magnetic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1b9tsbo</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>More Essie special effects line</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9tsbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1b9rhtu</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Cirque Brightside 🧡</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9rhtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1b9qwqz</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>🦩 Polishes Used: Cirque Colors (Shade: Flaminglow) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9qwqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1b9s90n</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Does anyone else find that A-England chips very quickly?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b9s90n/does_anyone_else_find_that_aengland_chips_very/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1b9rxog</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Any advice to make the glitter more full coverage on the tips?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8a0ola0wx4nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1b9ru2o</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>appreciation post for my bare nails, currently mourning the loss of my left middle and right pointer nails, with a deep tear in my left thumbnail :c</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9ru2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1b9ro9l</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Moss Magic 🌿</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w11moax3w4nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1b9rky5</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Not so proud of this one</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3eau3xygv4nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1b9q28e</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Unsure about the slight visible VNL but the color is 💯</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5vovshnk4nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1b9pqva</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>LynB sale?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b9pqva/lynb_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1b9pc7i</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Combined two randomly chosen colours</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9pc7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1b9mxzg</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Which nail wraps do you like best?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1b9mxzg/which_nail_wraps_do_you_like_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1b9mqzp</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Not another Pigeon post!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9mqzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1b9l7b0</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Cirque Lost Berry</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9l7b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1b9icqr</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>shades like this color?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evdq2c42c2nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1b9j4ym</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>China Glaze Too Yacht 2 Handle</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23dkjuwzk2nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ba8uc6</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>First time getting acrylic nails! What do you think?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba8uc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ba47yq</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>St. Patty Day Nails!</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2eoz4x6e7nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ba4603</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7vgrjdud7nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ba01mo</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>very messy first attempt! (+my cat :3)</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ba01mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1b9zr2n</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>I Did These Earlier And Am Really Happy With How They Came Out! 🖤🤍✨</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9zr2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1b9wvj3</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Just made a ring out of poly gel and strawberry nails 😍</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9wvj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1b9w2f8</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Squiggly〰️</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzodv3ovq5nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1b9q9zn</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Getting the hint of spring on my finger tips.</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9q9zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1b9nk89</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>First nailart attempt</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9nk89</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1b9kjti</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>These took good few days (I'm a beginner) tried polygel gel for the first time i NEED to know what's the longest time you ever did your nails as a beginner? I wanna know am I the only one sitting for straight 9 hours a day and then do the same the next day</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1b9kjti</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar 10 08:07:06 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_03_10.xlsx
+++ b/data/2024_03_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C971"/>
+  <dimension ref="A1:C1128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16940,6 +16940,2675 @@
         </is>
       </c>
     </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1bb4qgh</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Removable fake nails </t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bb4qgh/removable_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1bb3u9g</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Where can I find these star/heart decals and charms?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l2p408odgnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1bb33bu</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Missing my long natural nails</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h7n65hj5gnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1bb2yqo</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Painted these last night</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bb2yqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1bb2xxw</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>St Patrick’s lil frogs</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aovwhmgv3gnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1baz1io</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Fill??</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1baz1io/fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1bayhy2</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Brush on glue. How do I make that stuff last?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bayhy2/brush_on_glue_how_do_i_make_that_stuff_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1bb2shx</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Rosary nails first attempt</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8is9i3z82gnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1bb1kus</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Nail salon won't remove other salons' work – is this normal?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bb1kus/nail_salon_wont_remove_other_salons_work_is_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1bb16n0</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Tried gemstones for the first time.</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bb16n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1bb0b5b</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Velvet Magnet Nails</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h5aei04edfnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1bb0a2o</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>My go-to easy pink and white ombrè acrylic nails that go with everything! 💅🏼✨💕</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcbnz7t5dfnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1bazxj7</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Did my nails this week and just found this sub. Want to share my mani of the weeks!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bazxj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1bazx85</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Frenchy Chrome on natural nails by @studioxongles on IG🤍💅🧖</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bazx85</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1bazpzh</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Sparkly green nails</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fozmi5608fnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1bazbod</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>First time doing something other than straight color</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n16egm7a4fnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1bays6u</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Wanted to share them !</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nqwgtehzenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1bayluh</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>First time doing dip nails🥰</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjgzawrvxenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1bayi11</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Need advice for preparing press on nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bayi11</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1bay2ig</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Just the two of them (they can make if they try)</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvw8cpz4tenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1baxpe9</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Goal was rainbow, shamrock, pot of gold. Tried on my daughter first and then bailed but I still love it! (Ignore overpaint)</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baxpe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1bavnhx</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>First photo is what client wanted and the rest is what she got. (She didnt want the gems she preferred the sparkle) would you be happy?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bavnhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1bawe8x</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Springy nails 🐸🍓🌸</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4gktbwyeenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1baxa3p</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Polygel / Sculpting Gel As Jewelry Charms?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1baxa3p/polygel_sculpting_gel_as_jewelry_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1bax8nf</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Japanese style nails</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bax8nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1bax74x</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Strawberry cuties</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wh55o7nlenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1bax5av</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>St. Patty's nails ☘️</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uh9b5ug8lenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1bawubf</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>what are the factors you look for in a new nail salon?</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bawubf/what_are_the_factors_you_look_for_in_a_new_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1bawgli</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>This blue 😍💙</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bawgli</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1bavze5</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Holo/Iridescent glitter gel polish</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bavze5/holoiridescent_glitter_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1bavlhu</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Hard gel and loose glitter...yes I do them myself</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bavlhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1bav7io</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>one of my favorite nail colors ❤️</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bav7io</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1batod1</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Day 1 of strengthener and cuticle oil!!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7a8so4stdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1batbmw</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>One of my all time favorite sets</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzef41w1rdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1bat96j</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Madam Glam in Virgo</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ass1tuohqdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1bashg2</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>original kuromi design by me, done by gia at savvy nails &amp; spa!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5q43k3elkdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1bas91l</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Shape advice</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9u51jttidnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1barypp</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Really liking this BTArtbox press on nails</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p4u6v0fogdnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1barrli</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Wedding</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1barrli/wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1bare0v</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>extra short gel x!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvf8ki0ccdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1bar0r0</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥹🧁</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bar0r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1baqdxx</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Will they make me do a fill?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v42nlmu4dnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1baqc5f</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>just LOVE this color</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8n3tf0h4dnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1baqbt2</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>🥰</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uaj73eca4dnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1baq4n4</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baq4n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1bapb5z</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Is there a polish that can replicate this color? Nails by @toplinenails IG</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0y5qk2jjwcnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1bao5tv</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>what I got (@nailsbysandyyy) vs the inspiration (@riellnails)</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bao5tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1bamfsb</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>How to treat callus on proximal nail fold?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bamfsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1bap3nd</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Early St Patrick’s Day</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yf9f1pxxucnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1baowgp</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Mani with nail tios</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baowgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1baotxs</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Russian manicure</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baotxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ban3lk</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Stick-on recommendations?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ban3lk/stickon_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1baocv3</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>My favourite set ever 💚🤍</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fir0xsbfpcnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1bamtu9</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>i’m feeling witchy - peek the nail crack in the last slide</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bamtu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1banajt</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Cirque Colors: Rose Canyon</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1banajt/cirque_colors_rose_canyon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1bana0w</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Always liked the dark color</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73u40d9bhcnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1ban65z</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Fresh Manicure, Ready to Start My New Job Monday :)</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ban65z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1bampgr</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Are these gels too thick for a home manicure?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bampgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1bamn8w</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>My nail tech left NO CRUMBS</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv9aurdtccnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1bamd1e</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>The perfect spring purple 💜😍</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxoc7r4racnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1bamb5e</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urooia9dacnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1balvi2</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Loving the pink side of life</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaht8we37cnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1baigot</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Best nailart I think I've done.</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baigot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1balfaq</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>🧡</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikfthmtl3cnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1bal92j</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>🐸🩷✨</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bal92j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1bal74v</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>practice set i did a while ago 🍔💛</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bal74v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1bal2dx</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Easter nails!</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24siwypr0cnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1bal03o</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>If the UV/LED nail lamp doesn't have a reflective bottom layer, should I put aluminium foil underneath?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epexyotb0cnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1bakvp0</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>E-file repair help? Bits don't fit</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8rvs0vvdzbnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1bahxdv</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>How do I make these shorter</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j31prdemabnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1baiqrr</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Nail Extensions with Poly Gel</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bmfdi2thbnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1baia3i</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Trying to decide if I should keep the same shape</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baia3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1bahxtu</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Nail tech popped off 💫</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bahxtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1bahu9e</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting rubber gel! </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9kxwczs9bnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1baht1a</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Clear holographic foils on black gel?</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9dgh6ei9bnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1bahjrg</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Broken glass nailart with hologram foil</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bahjrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1bag839</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>almond and soft pink, sensilla nails from Saturday💖</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6mbysrptanc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1baeo8q</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>New March Set</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mjaygmfbanc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1baeg2r</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Spring nails I painted myself</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0mz1bks8anc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1bae9jx</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>First gel extension</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/og48qynm6anc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1bacw76</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Froggy nails 🐸</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oq4zq4emp9nc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1bb51d5</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Zoya Sparrow</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y9j6ka9rgnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1bb3n52</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Twisted Terracotta Tanzanite</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bb3n52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1bb3ffh</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>What's with "Gosman" nail polishes that are all over TikTok and YouTube?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1s8xv899gnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1bb2s4j</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">As Glowy as Lorraine </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bb2s4j/as_glowy_as_lorraine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1bb2fk9</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Not sure what I could possibly be doing wrong at this point...</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbwzqb0hyfnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1bb1sze</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>ILNP Flicker</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bb1sze</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1bb1bzz</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Thermals where cold is lighter than warm colour?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bb1bzz/thermals_where_cold_is_lighter_than_warm_colour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1bb03h3</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Why does my polish come out looking like the surface of a brain?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bb03h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1baz7xz</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>tried at-home French tips for the first time and im pretty happy with them!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9k68oazc3fnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1bayg49</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Melancholia</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plrmdrwewenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1bay293</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Asked for advice earlier - here's the result!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bay293</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1baxgkw</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Mini nail tattoos!</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baxgkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1baxeq2</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>When the lighting in the weed store is *chef's kiss*</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8ec1zofnenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1bax9gp</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Sister bought me a Jodsone Gel Nail Polish Kit</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddf7qjd7menc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1bax8mn</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Spring is here 😊 first skittle</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bax8mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1baw9nk</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>How to prevent nail breakage?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1baw9nk/how_to_prevent_nail_breakage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1bavuxp</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>So what’s a good base coat for thin feeble nails?</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bavuxp/so_whats_a_good_base_coat_for_thin_feeble_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1bavqgo</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>SPOILERS AHEAD: I purchased the Lumen Year of the Dragon 🐉mystery pack so you don’t have to</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bavqgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1bavjxv</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Opi combos for fair skin?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icetfkba8enc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1bav730</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>ILNP Teddy 🐻 ✨</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x85begof5enc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1bav2w9</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Weekend mani 💅</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl97ighk4enc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1baurvw</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Random polish I made years ago</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baurvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1baul2v</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unicorn Puke </t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz6z7n1t0enc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1bauk88</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Polishes similar to Cirque’s Introverde?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bauk88/polishes_similar_to_cirques_introverde/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1bauaf7</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Nina Ultra Pro — Space Case</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/msrry49iydnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1bau4h1</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Velvet nails are so hard to capture</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/71jgri49xdnc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1batz49</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>The shiftiness of it all</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfivhv52wdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1batx0f</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Holo Taco Mint Mojito</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyz4qnwlvdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1batfpg</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Dupe for this BKL prototype</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq5ytw0zrdnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1bat5p6</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>My first Color Club holo!</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qznjcjnqpdnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1bat3zl</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Toxic Sludge 💚💜</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bat3zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1basho0</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>I’m not sure I’m into white polish</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1basho0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1baryt1</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>How to paint with regular polish after using gel</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1baryt1/how_to_paint_with_regular_polish_after_using_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1barqex</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Spring Leaves</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1barqex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1bargtx</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Jelly rainbow and Hello Kitty stickers</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bargtx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1barggb</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Weirdly won over by this grungy gold, even though it isn't very "me"</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ji7aa7bucdnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1barca5</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Green and yellow 70’s vibes</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1barca5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1baqxdb</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Is winter done yet.. ready for some spring color 🌸🌼🌞💐</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1baqxdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1baoy1s</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Essie “rooting for you”</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1baoy1s/essie_rooting_for_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1baosj8</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>'Forest' by Absolute New York nail lacquer</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/FEMl1Bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1banhdr</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Using polish regularly was wrecking my nails</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1banhdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ban1sv</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Cadillaquer Northern Cardinal</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ban1sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ban173</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>All time favorite</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ban173</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1bamqq0</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>LynBdesigns Fair Isle</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bamqq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1bamjc7</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Tried to recreate Oceanic Forces with gel polish!</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8epd753zbcnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1bamgg8</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>ILNP High Voltage</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cpfuflebcnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1bam1xo</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where to find indie polish in London/Edinburgh? </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bam1xo/where_to_find_indie_polish_in_londonedinburgh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1baljnw</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Secret drugstore crellies?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1baljnw/secret_drugstore_crellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1bal16d</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Can someone help me find a dupe for Zoya's Portia?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bal16d/can_someone_help_me_find_a_dupe_for_zoyas_portia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1baksz9</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>I like QOTD way more than I expected to!</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a594yt1sybnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1bakoir</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>what's a ~blasephemous~ hot take you have on nails?</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bakoir/whats_a_blasephemous_hot_take_you_have_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1bakid7</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>They’re giving *teeth*</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jubttwqfwbnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1bakfmw</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Classic Red ❤️</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bakfmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1bak9t9</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Needy fuzzy paw</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bak9t9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1bak86i</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Matte Maroon Polish</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bak86i/matte_maroon_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1bajtmx</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Perfect match </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5iugmdwqbnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1bajkg1</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love this colour! </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s1uc2ouobnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1bah6jm</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Had a play around with layering thermals and shimmers</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bah6jm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1bb50hz</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>I'll call this Aurora "Lite" on black. The budget, express version that requires little to no skill... hence the results 🤣</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7icrbdhzqgnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1bb2t0i</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Gel nails turned yellow</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bb2t0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1bazyuf</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Frenchy Chrome on natural nails by @studioxongles on IG🤍💅🧖</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bazyuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1baz50e</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>First time trying something other than a straight color</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/waoh5o0o2fnc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1bax85v</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Japanese style nails</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bax85v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1bawf5a</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Acrylic nails with gold rhinestones</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k9kwwu5fenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1bawdaf</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>star girl nails🤩</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmkysyyqeenc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1bavfdl</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Modern salon almond. Gel with some flakes and a pistachio French and for the bonus, some stone design. I’m in love with this shape and also with this beautiful and photographable hands. What do you think? ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bavfdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1bav5b7</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>extra short gel x 🤍</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erxvq0y25enc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1bat3tj</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>We're all mad here...</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bum1x4qcpdnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1baqt7d</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>HAZBIN HOTEL nails</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5egl0ry7dnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1bap8ad</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Yay nails!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmpae0vyvcnc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1bamv2c</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>I was inspired by Smashing Pumpkins' "Melon Collie And The Infinite Sadness" album cover. ✨</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bamv2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1balsya</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Up hand painted press ons</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1balsya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1bakcyv</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>💐 spring floral nails</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bakcyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1bahkij</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Broken glass nailart with hologram foil</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bahkij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1bag35r</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>First time painting on such a teeny "canvas"</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bag35r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1baef7o</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Spring nails I painted myself</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2n1m5vh8anc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>